<commit_message>
Added store tier charts
</commit_message>
<xml_diff>
--- a/documents/storeCharts.xlsx
+++ b/documents/storeCharts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OWNER\dippa\dippa-teemup\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3741399D-3262-47DB-97C1-1CA8976CB870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF03045F-8055-45EC-985F-FB4047BA9B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CC41351E-E70F-494E-A51E-F384CA71C45B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{CC41351E-E70F-494E-A51E-F384CA71C45B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,31 +40,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
-    <t>Premium</t>
-  </si>
-  <si>
-    <t>Hot</t>
-  </si>
-  <si>
-    <t>Cool</t>
-  </si>
-  <si>
-    <t>Transaction optimized</t>
-  </si>
-  <si>
-    <t>Premium SSD</t>
-  </si>
-  <si>
     <t>SSD</t>
   </si>
   <si>
     <t>HDD</t>
   </si>
   <si>
-    <t>Cold</t>
+    <t>Kuuma</t>
   </si>
   <si>
-    <t>Archive</t>
+    <t>Arkisto</t>
+  </si>
+  <si>
+    <t>Viileä</t>
+  </si>
+  <si>
+    <t>Kylmä</t>
+  </si>
+  <si>
+    <t>Korkealuokkainen</t>
+  </si>
+  <si>
+    <t>Tapahtumaoptimoitu</t>
+  </si>
+  <si>
+    <t>Korkealuokkainen SSD</t>
   </si>
 </sst>
 </file>
@@ -158,7 +158,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Files -palvelun eri palvelumallejen kirjoitusnopeuksia tiedostoille </a:t>
+              <a:t> Filesin eri palvelumallejen kirjoitusnopeuksia tiedostoille </a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -230,16 +230,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Premium</c:v>
+                  <c:v>Korkealuokkainen</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Transaction optimized</c:v>
+                  <c:v>Tapahtumaoptimoitu</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Hot</c:v>
+                  <c:v>Kuuma</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Cool</c:v>
+                  <c:v>Viileä</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -293,16 +293,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Premium</c:v>
+                  <c:v>Korkealuokkainen</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Transaction optimized</c:v>
+                  <c:v>Tapahtumaoptimoitu</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Hot</c:v>
+                  <c:v>Kuuma</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Cool</c:v>
+                  <c:v>Viileä</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -635,7 +635,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Storage -palvelun eri palvelumallejen kirjoitusnopeuksia tiedostoille</a:t>
+              <a:t> Storagen eri palvelumallejen kirjoitusnopeuksia tiedostoille</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -702,16 +702,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Hot</c:v>
+                  <c:v>Kuuma</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Cool</c:v>
+                  <c:v>Viileä</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Cold</c:v>
+                  <c:v>Kylmä</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Archive</c:v>
+                  <c:v>Arkisto</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -765,16 +765,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Hot</c:v>
+                  <c:v>Kuuma</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Cool</c:v>
+                  <c:v>Viileä</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Cold</c:v>
+                  <c:v>Kylmä</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Archive</c:v>
+                  <c:v>Arkisto</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1107,7 +1107,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Disk -palvelun eri palvelumallejen kirjoitusnopeuksia tiedostoille </a:t>
+              <a:t> Diskin eri palvelumallejen kirjoitusnopeuksia tiedostoille </a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1171,7 +1171,7 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Premium SSD</c:v>
+                  <c:v>Korkealuokkainen SSD</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>SSD</c:v>
@@ -1228,7 +1228,7 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Premium SSD</c:v>
+                  <c:v>Korkealuokkainen SSD</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>SSD</c:v>
@@ -3603,7 +3603,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3613,7 +3613,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1">
         <v>2685</v>
@@ -3624,7 +3624,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>2721</v>
@@ -3635,7 +3635,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>2716</v>
@@ -3646,7 +3646,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>3559</v>
@@ -3665,8 +3665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E8E946D-2B9E-4C70-B352-C284F38F4C35}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3676,7 +3676,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1">
         <v>29.431999999999999</v>
@@ -3687,7 +3687,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>29.273</v>
@@ -3698,7 +3698,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>29.847000000000001</v>
@@ -3709,7 +3709,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>29.920999999999999</v>
@@ -3728,8 +3728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A545BE-914C-4184-8F7D-0CA9F8CF38A2}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3739,7 +3739,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B1">
         <v>386</v>
@@ -3750,7 +3750,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>417</v>
@@ -3761,7 +3761,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>821</v>

</xml_diff>

<commit_message>
Added store tier charts and Azure text
</commit_message>
<xml_diff>
--- a/documents/storeCharts.xlsx
+++ b/documents/storeCharts.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OWNER\dippa\dippa-teemup\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF03045F-8055-45EC-985F-FB4047BA9B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277162F9-2F22-4C5B-ABC9-49993E8B8042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{CC41351E-E70F-494E-A51E-F384CA71C45B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>SSD</t>
   </si>
@@ -153,12 +154,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Azure</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Filesin eri palvelumallejen kirjoitusnopeuksia tiedostoille </a:t>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Azure Files -palvelun eri palvelumallien kirjoitusnopeudet tiedostoille</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -630,17 +627,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Blob</a:t>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Blob Storage -palvelun eri palvelumallien kirjoitusnopeudet tiedostoille</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Storagen eri palvelumallejen kirjoitusnopeuksia tiedostoille</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1103,11 +1093,476 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Managed</a:t>
+              <a:t>Azure Files -palvelun 300 MB:n</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Diskin eri palvelumallejen kirjoitusnopeuksia tiedostoille </a:t>
+              <a:t> tiedoston tallentamisnopeudet eri redundanssi-alueilla</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>LRS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$1:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Korkealuokkainen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tapahtumaoptimoitu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kuuma</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Viileä</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$B$1:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2685</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2721</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2716</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3559</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3E10-45EF-B1FA-924AE5B02429}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ZRS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$1:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Korkealuokkainen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tapahtumaoptimoitu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kuuma</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Viileä</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$C$1:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2689</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2687</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2686</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2685</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3E10-45EF-B1FA-924AE5B02429}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="2013604399"/>
+        <c:axId val="2013619279"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2013604399"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2013619279"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2013619279"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>aika</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2013604399"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Managed Disk -palvelun eri palvelumallien kirjoitusnopeudet tiedostoille</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1645,6 +2100,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -2656,6 +3151,511 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3206,15 +4206,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>143826</xdr:rowOff>
+      <xdr:rowOff>136206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>41909</xdr:rowOff>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3243,6 +4243,47 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>159066</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00CF42D0-C98B-C454-2A0F-034FB1D902D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3603,7 +4644,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3666,7 +4707,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3725,11 +4766,71 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A1F7F8-3DAD-45A1-BA15-D8FB9C542044}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1">
+        <v>2685</v>
+      </c>
+      <c r="C1">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>2721</v>
+      </c>
+      <c r="C2">
+        <v>2687</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2716</v>
+      </c>
+      <c r="C3">
+        <v>2686</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3559</v>
+      </c>
+      <c r="C4">
+        <v>2685</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A545BE-914C-4184-8F7D-0CA9F8CF38A2}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added HTTP-version survey results
</commit_message>
<xml_diff>
--- a/documents/storeCharts.xlsx
+++ b/documents/storeCharts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OWNER\dippa\dippa-teemup\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CAE834-469C-44EF-947A-0059ADC25E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E3E7FE-471D-4D33-9FC2-DECC87BAF9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{CC41351E-E70F-494E-A51E-F384CA71C45B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{CC41351E-E70F-494E-A51E-F384CA71C45B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,15 @@
     <sheet name="wireShark200M" sheetId="13" r:id="rId5"/>
     <sheet name="Sheet12" sheetId="14" r:id="rId6"/>
     <sheet name="wireShark1M" sheetId="12" r:id="rId7"/>
-    <sheet name="Sheet11" sheetId="11" r:id="rId8"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId9"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId10"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId11"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId12"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId13"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId14"/>
+    <sheet name="Sheet13" sheetId="15" r:id="rId8"/>
+    <sheet name="Sheet14" sheetId="16" r:id="rId9"/>
+    <sheet name="Sheet11" sheetId="11" r:id="rId10"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId11"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId12"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId13"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId14"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId15"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="6" hidden="1">wireShark1M!$A$1:$B$8</definedName>
@@ -64,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>SSD</t>
   </si>
@@ -182,6 +184,21 @@
   <si>
     <t>Kirjoitus ja poisto</t>
   </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Cosmos</t>
+  </si>
+  <si>
+    <t>Azure Files</t>
+  </si>
+  <si>
+    <t>Blob Storage</t>
+  </si>
+  <si>
+    <t>Managed Disks</t>
+  </si>
 </sst>
 </file>
 
@@ -216,9 +233,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,8 +574,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>aika</a:t>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t>Aika</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
@@ -751,6 +767,1001 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>WebSocket-lähetyksen tiedoston kasvu</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet6!$A$1:$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>binary</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>string</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet6!$B$1:$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E5A3-4109-8A23-B4858B47CB6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="110461199"/>
+        <c:axId val="110461679"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="110461199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Siirrettävän datan formaatti</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="110461679"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="110461679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tiedoston kasvuprosentti (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="110461199"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>HTTP-lataus</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> eri pyyntöjen koolla ja koodauksilla</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>base64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$A$14:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5 kB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50 kB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500 kB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$B$14:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E33C-4365-A1FA-D7ADA91EBB7A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$C$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>array</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$A$14:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5 kB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50 kB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500 kB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$C$14:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E33C-4365-A1FA-D7ADA91EBB7A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$D$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>form-data</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$A$14:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5 kB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50 kB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500 kB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$D$14:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E33C-4365-A1FA-D7ADA91EBB7A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="913858191"/>
+        <c:axId val="913859151"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="913858191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t>HTTP-pyynnön koko</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="913859151"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="913859151"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t>Aika (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="913858191"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>HTTP-lataus</a:t>
             </a:r>
             <a:r>
@@ -1135,7 +2146,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1100" baseline="0"/>
-                  <a:t>Latausaika (s)</a:t>
+                  <a:t>Aika (s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1287,7 +2298,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1581,7 +2592,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1594,14 +2605,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>aika</a:t>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t>Aika (s)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (s)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1618,7 +2624,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1752,7 +2758,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2050,7 +3056,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2063,14 +3069,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>aika</a:t>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t>Aika (ms)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (ms)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2087,7 +3088,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2221,7 +3222,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2503,7 +3504,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2516,14 +3517,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>aika</a:t>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t>Aika (ms)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (ms)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2540,7 +3536,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -3611,7 +4607,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1100" baseline="0"/>
-                  <a:t>Latausaika (s)</a:t>
+                  <a:t>Aika (s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4083,7 +5079,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1100" baseline="0"/>
-                  <a:t>Latausaika (s)</a:t>
+                  <a:t>Aika (s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5660,419 +6656,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>WebSocket-lähetyksen tiedoston kasvu</a:t>
+              <a:t>FTP-, FTPS- ja SFTP-lataukset Python-koodi</a:t>
             </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet6!$A$1:$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>binary</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>string</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet6!$B$1:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>97</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E5A3-4109-8A23-B4858B47CB6A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="110461199"/>
-        <c:axId val="110461679"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="110461199"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Siirrettävän datan formaatti</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="110461679"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="110461679"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Tiedoston kasvuprosentti (%)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="110461199"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>HTTP-lataus</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> eri pyyntöjen koolla ja koodauksilla</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -6117,11 +6702,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet7!$B$13</c:f>
+              <c:f>Sheet13!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>base64</c:v>
+                  <c:v>FTP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6138,42 +6723,42 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet7!$A$14:$A$16</c:f>
+              <c:f>Sheet13!$B$7:$D$7</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5 kB</c:v>
+                  <c:v>1 kB</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50 kB</c:v>
+                  <c:v>1 MB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500 kB</c:v>
+                  <c:v>10 MB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet7!$B$14:$B$16</c:f>
+              <c:f>Sheet13!$B$8:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9000000000000004</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E33C-4365-A1FA-D7ADA91EBB7A}"/>
+              <c16:uniqueId val="{00000000-1099-44EB-93B5-C0A1AF2DADD9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6182,11 +6767,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet7!$C$13</c:f>
+              <c:f>Sheet13!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>array</c:v>
+                  <c:v>FTPS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6203,42 +6788,42 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet7!$A$14:$A$16</c:f>
+              <c:f>Sheet13!$B$7:$D$7</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5 kB</c:v>
+                  <c:v>1 kB</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50 kB</c:v>
+                  <c:v>1 MB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500 kB</c:v>
+                  <c:v>10 MB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet7!$C$14:$C$16</c:f>
+              <c:f>Sheet13!$B$9:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.4</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.7</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E33C-4365-A1FA-D7ADA91EBB7A}"/>
+              <c16:uniqueId val="{00000001-1099-44EB-93B5-C0A1AF2DADD9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6247,11 +6832,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet7!$D$13</c:f>
+              <c:f>Sheet13!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>form-data</c:v>
+                  <c:v>SFTP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6268,42 +6853,42 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet7!$A$14:$A$16</c:f>
+              <c:f>Sheet13!$B$7:$D$7</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5 kB</c:v>
+                  <c:v>1 kB</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50 kB</c:v>
+                  <c:v>1 MB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500 kB</c:v>
+                  <c:v>10 MB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet7!$D$14:$D$16</c:f>
+              <c:f>Sheet13!$B$10:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>29</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.2</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8</c:v>
+                  <c:v>22.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E33C-4365-A1FA-D7ADA91EBB7A}"/>
+              <c16:uniqueId val="{00000002-1099-44EB-93B5-C0A1AF2DADD9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6317,11 +6902,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="913858191"/>
-        <c:axId val="913859151"/>
+        <c:axId val="157826175"/>
+        <c:axId val="158221583"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="913858191"/>
+        <c:axId val="157826175"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6348,7 +6933,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1100" baseline="0"/>
-                  <a:t>HTTP-pyynnön koko</a:t>
+                  <a:t>Tiedoston koko</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6419,7 +7004,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="913859151"/>
+        <c:crossAx val="158221583"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6427,7 +7012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="913859151"/>
+        <c:axId val="158221583"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6468,7 +7053,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1100" baseline="0"/>
-                  <a:t>Latausaika (s)</a:t>
+                  <a:t> Aika (s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6533,7 +7118,631 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="913858191"/>
+        <c:crossAx val="157826175"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>FTP-, FTPS- ja SFTP-lataukset C#-koodi</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet13!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FTP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet13!$B$20:$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1 kB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet13!$B$21:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8499999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-805D-4672-A945-AD299A4D6CD3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet13!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FTPS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet13!$B$20:$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1 kB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet13!$B$22:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-805D-4672-A945-AD299A4D6CD3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet13!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SFTP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet13!$B$20:$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1 kB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 MB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10 MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet13!$B$23:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-805D-4672-A945-AD299A4D6CD3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="344122287"/>
+        <c:axId val="344115567"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="344122287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tiedoston</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> koko</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="344115567"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="344115567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t> Aika (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="344122287"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6781,6 +7990,86 @@
 </file>
 
 <file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -8149,7 +9438,7 @@
 </file>
 
 <file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -8353,23 +9642,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -8474,8 +9762,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -8607,20 +9895,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -8654,7 +9941,7 @@
 </file>
 
 <file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -8858,6 +10145,509 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -9158,7 +10948,512 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13733,6 +16028,47 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
+      <xdr:colOff>169545</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>21908</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>474345</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F566D21-212D-61CC-4973-1D196CAF73CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>366712</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
@@ -13769,7 +16105,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -13810,7 +16146,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -13851,7 +16187,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -14142,6 +16478,83 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2FAF5FE-5352-A69D-8590-50F0B4C9ED1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2281573C-ECEA-796A-7C83-334ABEAD4AA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>427672</xdr:colOff>
       <xdr:row>11</xdr:row>
@@ -14159,47 +16572,6 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC661D8D-0F51-DB02-F281-EF7DB8010CE9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>169545</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>21908</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>474345</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F566D21-212D-61CC-4973-1D196CAF73CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14246,7 +16618,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9D63BC7D-F89D-4252-A309-28EAA8E44FA7}" name="wireShark200M" displayName="wireShark200M" ref="A1:B8" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B8" xr:uid="{9D63BC7D-F89D-4252-A309-28EAA8E44FA7}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8CA45A79-B873-4F69-A9E3-FC79AF039F00}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{8CA45A79-B873-4F69-A9E3-FC79AF039F00}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{6207EF3A-DEDE-46F4-BB64-94A37751C3B2}" uniqueName="2" name="Column2" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -14257,7 +16629,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F098AAA-1E61-4C06-AB36-156B43578C04}" name="wireShark1M" displayName="wireShark1M" ref="A1:B8" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B8" xr:uid="{3F098AAA-1E61-4C06-AB36-156B43578C04}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{620CE11D-5214-4C01-8C18-64DE761B37C8}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{620CE11D-5214-4C01-8C18-64DE761B37C8}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{E075A4D0-2535-435D-BC8C-2524E3D42A62}" uniqueName="2" name="Column2" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -14584,7 +16956,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14643,6 +17015,50 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175EC6FC-9A80-4235-BE10-EAD00CDF9ACB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5829646-3FDE-4A49-93D3-8D566EF74358}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874920F2-4AF6-439B-AEA0-E607796AE4D4}">
   <dimension ref="A13:D16"/>
   <sheetViews>
@@ -14714,7 +17130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D2AE20-1EB0-419A-B38B-6D581E61311C}">
   <dimension ref="A4:C7"/>
   <sheetViews>
@@ -14774,7 +17190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E8E946D-2B9E-4C70-B352-C284F38F4C35}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -14837,7 +17253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A1F7F8-3DAD-45A1-BA15-D8FB9C542044}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -14897,7 +17313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A545BE-914C-4184-8F7D-0CA9F8CF38A2}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -15206,7 +17622,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2">
@@ -15214,7 +17630,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>26</v>
       </c>
       <c r="B3">
@@ -15222,7 +17638,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4">
@@ -15230,7 +17646,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>28</v>
       </c>
       <c r="B5">
@@ -15238,7 +17654,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6">
@@ -15246,7 +17662,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="B7">
@@ -15254,7 +17670,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
       <c r="B8">
@@ -15274,7 +17690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA8B274-9715-4060-BF83-E7E2AAEB93C5}">
   <dimension ref="A5:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -15334,7 +17750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134663F2-2A32-4322-948E-2D3796F2D084}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -15353,7 +17769,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2">
@@ -15361,7 +17777,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>26</v>
       </c>
       <c r="B3">
@@ -15369,7 +17785,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4">
@@ -15377,7 +17793,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>28</v>
       </c>
       <c r="B5">
@@ -15385,7 +17801,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6">
@@ -15393,7 +17809,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="B7">
@@ -15401,7 +17817,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
       <c r="B8">
@@ -15418,46 +17834,193 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175EC6FC-9A80-4235-BE10-EAD00CDF9ACB}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{779B51D2-9B60-4FDA-A659-E126E1C32A60}">
+  <dimension ref="A7:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>1.8</v>
+      </c>
+      <c r="C8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D8">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>2.4</v>
+      </c>
+      <c r="C9">
+        <v>3.1</v>
+      </c>
+      <c r="D9">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10">
+        <v>2.4</v>
+      </c>
+      <c r="C10">
+        <v>4.7</v>
+      </c>
+      <c r="D10">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>1.9</v>
+      </c>
+      <c r="C21">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D21">
+        <v>4.8499999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>2.4</v>
+      </c>
+      <c r="C22">
+        <v>3.1</v>
+      </c>
+      <c r="D22">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C23">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D23">
+        <v>12.1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5829646-3FDE-4A49-93D3-8D566EF74358}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA22D98D-70C3-4BBD-A2AA-F77EEE824602}">
+  <dimension ref="A8:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1">
-        <v>11</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2">
-        <v>97</v>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9">
+        <v>0.3</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>